<commit_message>
Update job titles to Software Developer, SRE, and Engineering Manager
Changed sample data job titles from Product Manager/Data roles to be
compatible with engineering team structure: Software Developers, SREs,
and Engineering Managers.

Changes:
- Updated create_sample_data.py with engineering-focused job titles
- Small team: 12 employees (Software Developers & SREs) under 1 manager
- Large org: 50 employees including Engineering Managers (Director-level view)
- Large org simulates Director rating their managers and IC contributors
- Regenerated sample-data-large.xlsx with new titles
- Updated README.md to clarify use-cases for small vs large datasets

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data-large.xlsx
+++ b/sample-data-large.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Principal Engineer</t>
+          <t>Principal Software Developer</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -557,9 +557,6 @@
       <c r="K3" t="n">
         <v>20</v>
       </c>
-      <c r="L3" t="n">
-        <v>110</v>
-      </c>
       <c r="M3" t="n">
         <v>44000</v>
       </c>
@@ -579,7 +576,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Staff Engineer</t>
+          <t>Engineering Manager</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -590,7 +587,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>180000</v>
+        <v>190000</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -599,17 +596,17 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>IC4</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L4" t="n">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="M4" t="n">
-        <v>27000</v>
+        <v>34200</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
@@ -627,7 +624,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Staff Software Developer</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -638,7 +635,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>150000</v>
+        <v>180000</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -647,14 +644,17 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC4</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="L5" t="n">
+        <v>115</v>
       </c>
       <c r="M5" t="n">
-        <v>18000</v>
+        <v>27000</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
@@ -672,7 +672,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>145000</v>
+        <v>150000</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -699,10 +699,10 @@
         <v>12</v>
       </c>
       <c r="L6" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="M6" t="n">
-        <v>17400</v>
+        <v>18000</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
@@ -720,7 +720,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -731,7 +731,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>120000</v>
+        <v>145000</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -740,17 +740,14 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>IC2</t>
+          <t>IC3</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>10</v>
-      </c>
-      <c r="L7" t="n">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="M7" t="n">
-        <v>12000</v>
+        <v>17400</v>
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
@@ -768,7 +765,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -779,7 +776,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>115000</v>
+        <v>120000</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -795,10 +792,10 @@
         <v>10</v>
       </c>
       <c r="L8" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="M8" t="n">
-        <v>11500</v>
+        <v>12000</v>
       </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
@@ -816,7 +813,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -827,7 +824,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>118000</v>
+        <v>115000</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -843,10 +840,10 @@
         <v>10</v>
       </c>
       <c r="L9" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="M9" t="n">
-        <v>11800</v>
+        <v>11500</v>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
@@ -864,7 +861,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -875,7 +872,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>112000</v>
+        <v>118000</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -890,11 +887,8 @@
       <c r="K10" t="n">
         <v>10</v>
       </c>
-      <c r="L10" t="n">
-        <v>100</v>
-      </c>
       <c r="M10" t="n">
-        <v>11200</v>
+        <v>11800</v>
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
@@ -912,7 +906,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -923,7 +917,7 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>148000</v>
+        <v>112000</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -932,17 +926,17 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L11" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M11" t="n">
-        <v>17760</v>
+        <v>11200</v>
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
@@ -960,7 +954,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -987,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="L12" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="M12" t="n">
         <v>18240</v>
@@ -1008,7 +1002,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Staff Engineer</t>
+          <t>Staff Software Developer</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1035,7 +1029,7 @@
         <v>15</v>
       </c>
       <c r="L13" t="n">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="M13" t="n">
         <v>26250</v>
@@ -1056,7 +1050,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Engineering Manager</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1067,7 +1061,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>155000</v>
+        <v>185000</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1076,14 +1070,17 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="L14" t="n">
+        <v>105</v>
       </c>
       <c r="M14" t="n">
-        <v>18600</v>
+        <v>33300</v>
       </c>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
@@ -1101,7 +1098,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1112,7 +1109,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>149000</v>
+        <v>155000</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1127,11 +1124,8 @@
       <c r="K15" t="n">
         <v>12</v>
       </c>
-      <c r="L15" t="n">
-        <v>105</v>
-      </c>
       <c r="M15" t="n">
-        <v>17880</v>
+        <v>18600</v>
       </c>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
@@ -1149,7 +1143,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1160,7 +1154,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>110000</v>
+        <v>149000</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1169,14 +1163,17 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>IC2</t>
+          <t>IC3</t>
         </is>
       </c>
       <c r="K16" t="n">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="L16" t="n">
+        <v>115</v>
       </c>
       <c r="M16" t="n">
-        <v>11000</v>
+        <v>17880</v>
       </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
@@ -1194,7 +1191,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -1205,7 +1202,7 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>125000</v>
+        <v>110000</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1221,10 +1218,10 @@
         <v>10</v>
       </c>
       <c r="L17" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="M17" t="n">
-        <v>12500</v>
+        <v>11000</v>
       </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
@@ -1242,7 +1239,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -1253,7 +1250,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>147000</v>
+        <v>125000</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1262,17 +1259,17 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K18" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L18" t="n">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="M18" t="n">
-        <v>17640</v>
+        <v>12500</v>
       </c>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
@@ -1290,7 +1287,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -1301,7 +1298,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>122000</v>
+        <v>147000</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1310,17 +1307,17 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>IC2</t>
+          <t>IC3</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L19" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="M19" t="n">
-        <v>12200</v>
+        <v>17640</v>
       </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
@@ -1338,7 +1335,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -1349,7 +1346,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>151000</v>
+        <v>122000</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1358,17 +1355,14 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>12</v>
-      </c>
-      <c r="L20" t="n">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="M20" t="n">
-        <v>18120</v>
+        <v>12200</v>
       </c>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
@@ -1386,7 +1380,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -1412,9 +1406,6 @@
       <c r="K21" t="n">
         <v>10</v>
       </c>
-      <c r="L21" t="n">
-        <v>100</v>
-      </c>
       <c r="M21" t="n">
         <v>11900</v>
       </c>
@@ -1434,7 +1425,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -1460,9 +1451,6 @@
       <c r="K22" t="n">
         <v>10</v>
       </c>
-      <c r="L22" t="n">
-        <v>110</v>
-      </c>
       <c r="M22" t="n">
         <v>11600</v>
       </c>
@@ -1477,12 +1465,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Senior Product Manager</t>
+          <t>Principal Software Developer</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -1493,7 +1481,7 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>165000</v>
+        <v>215000</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1502,17 +1490,14 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>IC4</t>
+          <t>IC5</t>
         </is>
       </c>
       <c r="K23" t="n">
-        <v>15</v>
-      </c>
-      <c r="L23" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="M23" t="n">
-        <v>24750</v>
+        <v>43000</v>
       </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
@@ -1525,12 +1510,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Senior Product Manager</t>
+          <t>Staff Software Developer</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -1541,7 +1526,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>160000</v>
+        <v>182000</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1556,8 +1541,11 @@
       <c r="K24" t="n">
         <v>15</v>
       </c>
+      <c r="L24" t="n">
+        <v>110</v>
+      </c>
       <c r="M24" t="n">
-        <v>24000</v>
+        <v>27300</v>
       </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
@@ -1570,12 +1558,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Engineering Manager</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -1586,7 +1574,7 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>130000</v>
+        <v>188000</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1595,14 +1583,17 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="L25" t="n">
+        <v>85</v>
       </c>
       <c r="M25" t="n">
-        <v>15600</v>
+        <v>33840</v>
       </c>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
@@ -1615,12 +1606,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -1631,7 +1622,7 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>125000</v>
+        <v>158000</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1650,7 +1641,7 @@
         <v>90</v>
       </c>
       <c r="M26" t="n">
-        <v>15000</v>
+        <v>18960</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
@@ -1663,12 +1654,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -1679,7 +1670,7 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>135000</v>
+        <v>152000</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1694,8 +1685,11 @@
       <c r="K27" t="n">
         <v>12</v>
       </c>
+      <c r="L27" t="n">
+        <v>95</v>
+      </c>
       <c r="M27" t="n">
-        <v>16200</v>
+        <v>18240</v>
       </c>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
@@ -1708,12 +1702,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -1733,17 +1727,14 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>12</v>
-      </c>
-      <c r="L28" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="M28" t="n">
-        <v>15360</v>
+        <v>12800</v>
       </c>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
@@ -1756,12 +1747,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Senior Product Manager</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -1772,7 +1763,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>158000</v>
+        <v>122000</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1781,17 +1772,14 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>IC4</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K29" t="n">
-        <v>15</v>
-      </c>
-      <c r="L29" t="n">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="M29" t="n">
-        <v>23700</v>
+        <v>12200</v>
       </c>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
@@ -1804,12 +1792,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -1820,7 +1808,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>132000</v>
+        <v>118000</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1829,14 +1817,17 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K30" t="n">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="L30" t="n">
+        <v>100</v>
       </c>
       <c r="M30" t="n">
-        <v>15840</v>
+        <v>11800</v>
       </c>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
@@ -1849,12 +1840,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -1865,7 +1856,7 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>127000</v>
+        <v>155000</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1881,7 +1872,7 @@
         <v>12</v>
       </c>
       <c r="M31" t="n">
-        <v>15240</v>
+        <v>18600</v>
       </c>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
@@ -1894,12 +1885,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>Engineering - Backend Services</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -1910,7 +1901,7 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>133000</v>
+        <v>125000</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -1919,17 +1910,17 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K32" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L32" t="n">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="M32" t="n">
-        <v>15960</v>
+        <v>12500</v>
       </c>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr"/>
@@ -1942,12 +1933,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Senior Data Engineer</t>
+          <t>Senior SRE</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -1976,6 +1967,9 @@
       <c r="K33" t="n">
         <v>12</v>
       </c>
+      <c r="L33" t="n">
+        <v>90</v>
+      </c>
       <c r="M33" t="n">
         <v>12600</v>
       </c>
@@ -1993,12 +1987,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -2028,7 +2022,7 @@
         <v>10</v>
       </c>
       <c r="L34" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M34" t="n">
         <v>7800</v>
@@ -2047,12 +2041,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Senior Data Engineer</t>
+          <t>Staff SRE</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -2063,7 +2057,7 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>145000</v>
+        <v>185000</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -2072,17 +2066,17 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC4</t>
         </is>
       </c>
       <c r="K35" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L35" t="n">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="M35" t="n">
-        <v>17400</v>
+        <v>27750</v>
       </c>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr"/>
@@ -2095,12 +2089,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>Engineering Manager</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -2111,7 +2105,7 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>115000</v>
+        <v>192000</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -2120,17 +2114,17 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>IC2</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="K36" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L36" t="n">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="M36" t="n">
-        <v>11500</v>
+        <v>34560</v>
       </c>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
@@ -2143,12 +2137,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Senior Data Engineer</t>
+          <t>Senior SRE</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -2159,7 +2153,7 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>148000</v>
+        <v>155000</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2174,8 +2168,11 @@
       <c r="K37" t="n">
         <v>12</v>
       </c>
+      <c r="L37" t="n">
+        <v>115</v>
+      </c>
       <c r="M37" t="n">
-        <v>17760</v>
+        <v>18600</v>
       </c>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr"/>
@@ -2188,12 +2185,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>Senior SRE</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -2204,7 +2201,7 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>118000</v>
+        <v>152000</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -2213,17 +2210,17 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>IC2</t>
+          <t>IC3</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L38" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="M38" t="n">
-        <v>11800</v>
+        <v>18240</v>
       </c>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr"/>
@@ -2236,12 +2233,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Senior Data Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -2252,7 +2249,7 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>142000</v>
+        <v>125000</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2261,17 +2258,17 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K39" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L39" t="n">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="M39" t="n">
-        <v>17040</v>
+        <v>12500</v>
       </c>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr"/>
@@ -2284,12 +2281,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -2300,7 +2297,7 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>112000</v>
+        <v>122000</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -2316,10 +2313,10 @@
         <v>10</v>
       </c>
       <c r="L40" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M40" t="n">
-        <v>11200</v>
+        <v>12200</v>
       </c>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr"/>
@@ -2332,12 +2329,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Senior Data Engineer</t>
+          <t>Senior SRE</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -2348,7 +2345,7 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>150000</v>
+        <v>148000</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2363,8 +2360,11 @@
       <c r="K41" t="n">
         <v>12</v>
       </c>
+      <c r="L41" t="n">
+        <v>105</v>
+      </c>
       <c r="M41" t="n">
-        <v>18000</v>
+        <v>17760</v>
       </c>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr"/>
@@ -2377,12 +2377,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Engineering - Data</t>
+          <t>Engineering - Infrastructure</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>120000</v>
+        <v>130000</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -2408,8 +2408,11 @@
       <c r="K42" t="n">
         <v>10</v>
       </c>
+      <c r="L42" t="n">
+        <v>115</v>
+      </c>
       <c r="M42" t="n">
-        <v>12000</v>
+        <v>13000</v>
       </c>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr"/>
@@ -2422,12 +2425,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Staff Infrastructure Engineer</t>
+          <t>Staff SRE</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -2438,7 +2441,7 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>185000</v>
+        <v>188000</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2454,10 +2457,10 @@
         <v>15</v>
       </c>
       <c r="L43" t="n">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="M43" t="n">
-        <v>27750</v>
+        <v>28200</v>
       </c>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
@@ -2470,12 +2473,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Senior DevOps Engineer</t>
+          <t>Engineering Manager</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -2486,7 +2489,7 @@
         </is>
       </c>
       <c r="G44" t="n">
-        <v>155000</v>
+        <v>195000</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2495,17 +2498,17 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="K44" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="L44" t="n">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="M44" t="n">
-        <v>18600</v>
+        <v>35100</v>
       </c>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr"/>
@@ -2518,12 +2521,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Senior DevOps Engineer</t>
+          <t>Senior SRE</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -2534,7 +2537,7 @@
         </is>
       </c>
       <c r="G45" t="n">
-        <v>152000</v>
+        <v>160000</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2550,7 +2553,7 @@
         <v>12</v>
       </c>
       <c r="M45" t="n">
-        <v>18240</v>
+        <v>19200</v>
       </c>
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr"/>
@@ -2563,12 +2566,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>DevOps Engineer</t>
+          <t>Senior SRE</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -2579,7 +2582,7 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>125000</v>
+        <v>156000</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -2588,14 +2591,17 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>IC2</t>
+          <t>IC3</t>
         </is>
       </c>
       <c r="K46" t="n">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="L46" t="n">
+        <v>105</v>
       </c>
       <c r="M46" t="n">
-        <v>12500</v>
+        <v>18720</v>
       </c>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr"/>
@@ -2608,12 +2614,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>DevOps Engineer</t>
+          <t>Senior SRE</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -2624,7 +2630,7 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>122000</v>
+        <v>153000</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2633,17 +2639,14 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>IC2</t>
+          <t>IC3</t>
         </is>
       </c>
       <c r="K47" t="n">
-        <v>10</v>
-      </c>
-      <c r="L47" t="n">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="M47" t="n">
-        <v>12200</v>
+        <v>18360</v>
       </c>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr"/>
@@ -2656,12 +2659,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Senior Security Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
@@ -2672,7 +2675,7 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>160000</v>
+        <v>128000</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -2681,17 +2684,14 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K48" t="n">
-        <v>12</v>
-      </c>
-      <c r="L48" t="n">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="M48" t="n">
-        <v>19200</v>
+        <v>12800</v>
       </c>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr"/>
@@ -2704,12 +2704,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Security Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
@@ -2720,7 +2720,7 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>135000</v>
+        <v>124000</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>10</v>
       </c>
       <c r="M49" t="n">
-        <v>13500</v>
+        <v>12400</v>
       </c>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr"/>
@@ -2749,12 +2749,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Senior DevOps Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>148000</v>
+        <v>120000</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -2774,17 +2774,14 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>IC3</t>
+          <t>IC2</t>
         </is>
       </c>
       <c r="K50" t="n">
-        <v>12</v>
-      </c>
-      <c r="L50" t="n">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="M50" t="n">
-        <v>17760</v>
+        <v>12000</v>
       </c>
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr"/>
@@ -2797,12 +2794,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>DevOps Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
@@ -2813,7 +2810,7 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>128000</v>
+        <v>118000</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -2829,10 +2826,10 @@
         <v>10</v>
       </c>
       <c r="L51" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M51" t="n">
-        <v>12800</v>
+        <v>11800</v>
       </c>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr"/>
@@ -2845,12 +2842,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Engineering - Infrastructure</t>
+          <t>Engineering - Reliability</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>DevOps Engineer</t>
+          <t>SRE</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
@@ -2861,7 +2858,7 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>130000</v>
+        <v>115000</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
@@ -2877,7 +2874,7 @@
         <v>10</v>
       </c>
       <c r="M52" t="n">
-        <v>13000</v>
+        <v>11500</v>
       </c>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr"/>

</xml_diff>

<commit_message>
Change bonus targets from annual to quarterly percentages
Updated all bonus target percentages to be quarterly instead of annual
to match realistic quarterly performance review cycles.

Changes:
- IC2: 10% → 2.5% (quarterly)
- IC3: 12% → 3.0% (quarterly)
- IC4: 15% → 3.75% (quarterly)
- IC5: 20% → 5.0% (quarterly)
- M3: 18% → 4.5% (quarterly)

Examples:
- IC2 ($120K base): $3,000 quarterly ($12,000 annual)
- IC3 ($150K base): $4,500 quarterly ($18,000 annual)
- IC4 ($180K base): $6,750 quarterly ($27,000 annual)
- IC5 ($220K base): $11,000 quarterly ($44,000 annual)
- M3 ($190K base): $8,550 quarterly ($34,200 annual)

This makes the bonus amounts more realistic for quarterly reviews
while maintaining the same annual targets when multiplied by 4.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data-large.xlsx
+++ b/sample-data-large.xlsx
@@ -560,13 +560,13 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="L3" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="M3" t="n">
-        <v>44000</v>
+        <v>11000</v>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
@@ -611,10 +611,13 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>18</v>
+        <v>4.5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>90</v>
       </c>
       <c r="M4" t="n">
-        <v>34200</v>
+        <v>8550</v>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
@@ -659,13 +662,13 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>15</v>
+        <v>3.75</v>
       </c>
       <c r="L5" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M5" t="n">
-        <v>27000</v>
+        <v>6750</v>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
@@ -710,10 +713,13 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
+        <v>85</v>
       </c>
       <c r="M6" t="n">
-        <v>18000</v>
+        <v>4500</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
@@ -758,13 +764,13 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L7" t="n">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="M7" t="n">
-        <v>17400</v>
+        <v>4350</v>
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
@@ -809,10 +815,13 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>10</v>
+        <v>2.5</v>
+      </c>
+      <c r="L8" t="n">
+        <v>115</v>
       </c>
       <c r="M8" t="n">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
@@ -857,10 +866,13 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>10</v>
+        <v>2.5</v>
+      </c>
+      <c r="L9" t="n">
+        <v>100</v>
       </c>
       <c r="M9" t="n">
-        <v>11500</v>
+        <v>2875</v>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
@@ -905,13 +917,10 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>10</v>
-      </c>
-      <c r="L10" t="n">
-        <v>115</v>
+        <v>2.5</v>
       </c>
       <c r="M10" t="n">
-        <v>11800</v>
+        <v>2950</v>
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
@@ -956,13 +965,13 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L11" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="M11" t="n">
-        <v>11200</v>
+        <v>2800</v>
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
@@ -1007,10 +1016,10 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="M12" t="n">
-        <v>18240</v>
+        <v>4560</v>
       </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
@@ -1055,13 +1064,13 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>15</v>
+        <v>3.75</v>
       </c>
       <c r="L13" t="n">
         <v>90</v>
       </c>
       <c r="M13" t="n">
-        <v>26250</v>
+        <v>6562.5</v>
       </c>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
@@ -1106,13 +1115,13 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>18</v>
+        <v>4.5</v>
       </c>
       <c r="L14" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="M14" t="n">
-        <v>33300</v>
+        <v>8325</v>
       </c>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
@@ -1157,13 +1166,13 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L15" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M15" t="n">
-        <v>18600</v>
+        <v>4650</v>
       </c>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
@@ -1208,10 +1217,13 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="L16" t="n">
+        <v>110</v>
       </c>
       <c r="M16" t="n">
-        <v>17880</v>
+        <v>4470</v>
       </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
@@ -1256,10 +1268,13 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>10</v>
+        <v>2.5</v>
+      </c>
+      <c r="L17" t="n">
+        <v>100</v>
       </c>
       <c r="M17" t="n">
-        <v>11000</v>
+        <v>2750</v>
       </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
@@ -1304,13 +1319,13 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L18" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="M18" t="n">
-        <v>12500</v>
+        <v>3125</v>
       </c>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
@@ -1355,13 +1370,13 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L19" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="M19" t="n">
-        <v>17640</v>
+        <v>4410</v>
       </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
@@ -1406,13 +1421,13 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L20" t="n">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="M20" t="n">
-        <v>12200</v>
+        <v>3050</v>
       </c>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
@@ -1457,10 +1472,13 @@
         </is>
       </c>
       <c r="K21" t="n">
-        <v>10</v>
+        <v>2.5</v>
+      </c>
+      <c r="L21" t="n">
+        <v>105</v>
       </c>
       <c r="M21" t="n">
-        <v>11900</v>
+        <v>2975</v>
       </c>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
@@ -1505,10 +1523,13 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>10</v>
+        <v>2.5</v>
+      </c>
+      <c r="L22" t="n">
+        <v>110</v>
       </c>
       <c r="M22" t="n">
-        <v>11600</v>
+        <v>2900</v>
       </c>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
@@ -1553,10 +1574,13 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="L23" t="n">
+        <v>85</v>
       </c>
       <c r="M23" t="n">
-        <v>43000</v>
+        <v>10750</v>
       </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
@@ -1601,13 +1625,13 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>15</v>
+        <v>3.75</v>
       </c>
       <c r="L24" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M24" t="n">
-        <v>27300</v>
+        <v>6825</v>
       </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
@@ -1652,10 +1676,10 @@
         </is>
       </c>
       <c r="K25" t="n">
-        <v>18</v>
+        <v>4.5</v>
       </c>
       <c r="M25" t="n">
-        <v>33840</v>
+        <v>8460</v>
       </c>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
@@ -1700,10 +1724,13 @@
         </is>
       </c>
       <c r="K26" t="n">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="L26" t="n">
+        <v>90</v>
       </c>
       <c r="M26" t="n">
-        <v>18960</v>
+        <v>4740</v>
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
@@ -1748,13 +1775,13 @@
         </is>
       </c>
       <c r="K27" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L27" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M27" t="n">
-        <v>18240</v>
+        <v>4560</v>
       </c>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
@@ -1799,13 +1826,13 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L28" t="n">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="M28" t="n">
-        <v>12800</v>
+        <v>3200</v>
       </c>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
@@ -1850,13 +1877,13 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L29" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M29" t="n">
-        <v>12200</v>
+        <v>3050</v>
       </c>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
@@ -1901,13 +1928,13 @@
         </is>
       </c>
       <c r="K30" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L30" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M30" t="n">
-        <v>11800</v>
+        <v>2950</v>
       </c>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
@@ -1952,13 +1979,13 @@
         </is>
       </c>
       <c r="K31" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L31" t="n">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="M31" t="n">
-        <v>18600</v>
+        <v>4650</v>
       </c>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
@@ -2003,13 +2030,13 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L32" t="n">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="M32" t="n">
-        <v>12500</v>
+        <v>3125</v>
       </c>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr"/>
@@ -2057,16 +2084,13 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>12</v>
-      </c>
-      <c r="L33" t="n">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="M33" t="n">
-        <v>12600</v>
+        <v>3150</v>
       </c>
       <c r="N33" t="n">
-        <v>15949.32</v>
+        <v>3987.33</v>
       </c>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
@@ -2114,13 +2138,16 @@
         </is>
       </c>
       <c r="K34" t="n">
-        <v>10</v>
+        <v>2.5</v>
+      </c>
+      <c r="L34" t="n">
+        <v>110</v>
       </c>
       <c r="M34" t="n">
-        <v>7800</v>
+        <v>1950</v>
       </c>
       <c r="N34" t="n">
-        <v>9873.400000000001</v>
+        <v>2468.35</v>
       </c>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
@@ -2165,13 +2192,13 @@
         </is>
       </c>
       <c r="K35" t="n">
-        <v>15</v>
+        <v>3.75</v>
       </c>
       <c r="L35" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M35" t="n">
-        <v>27750</v>
+        <v>6937.5</v>
       </c>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr"/>
@@ -2216,10 +2243,13 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>18</v>
+        <v>4.5</v>
+      </c>
+      <c r="L36" t="n">
+        <v>95</v>
       </c>
       <c r="M36" t="n">
-        <v>34560</v>
+        <v>8640</v>
       </c>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
@@ -2264,13 +2294,13 @@
         </is>
       </c>
       <c r="K37" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L37" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="M37" t="n">
-        <v>18600</v>
+        <v>4650</v>
       </c>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr"/>
@@ -2315,13 +2345,13 @@
         </is>
       </c>
       <c r="K38" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L38" t="n">
         <v>115</v>
       </c>
       <c r="M38" t="n">
-        <v>18240</v>
+        <v>4560</v>
       </c>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr"/>
@@ -2366,10 +2396,10 @@
         </is>
       </c>
       <c r="K39" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="M39" t="n">
-        <v>12500</v>
+        <v>3125</v>
       </c>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr"/>
@@ -2414,13 +2444,13 @@
         </is>
       </c>
       <c r="K40" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L40" t="n">
         <v>90</v>
       </c>
       <c r="M40" t="n">
-        <v>12200</v>
+        <v>3050</v>
       </c>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr"/>
@@ -2465,13 +2495,13 @@
         </is>
       </c>
       <c r="K41" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L41" t="n">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="M41" t="n">
-        <v>17760</v>
+        <v>4440</v>
       </c>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr"/>
@@ -2516,13 +2546,10 @@
         </is>
       </c>
       <c r="K42" t="n">
-        <v>10</v>
-      </c>
-      <c r="L42" t="n">
-        <v>90</v>
+        <v>2.5</v>
       </c>
       <c r="M42" t="n">
-        <v>13000</v>
+        <v>3250</v>
       </c>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr"/>
@@ -2567,13 +2594,13 @@
         </is>
       </c>
       <c r="K43" t="n">
-        <v>15</v>
+        <v>3.75</v>
       </c>
       <c r="L43" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="M43" t="n">
-        <v>28200</v>
+        <v>7050</v>
       </c>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
@@ -2618,13 +2645,13 @@
         </is>
       </c>
       <c r="K44" t="n">
-        <v>18</v>
+        <v>4.5</v>
       </c>
       <c r="L44" t="n">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="M44" t="n">
-        <v>35100</v>
+        <v>8775</v>
       </c>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr"/>
@@ -2669,13 +2696,13 @@
         </is>
       </c>
       <c r="K45" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L45" t="n">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="M45" t="n">
-        <v>19200</v>
+        <v>4800</v>
       </c>
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr"/>
@@ -2720,13 +2747,13 @@
         </is>
       </c>
       <c r="K46" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L46" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="M46" t="n">
-        <v>18720</v>
+        <v>4680</v>
       </c>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr"/>
@@ -2771,13 +2798,13 @@
         </is>
       </c>
       <c r="K47" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L47" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="M47" t="n">
-        <v>18360</v>
+        <v>4590</v>
       </c>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr"/>
@@ -2822,10 +2849,13 @@
         </is>
       </c>
       <c r="K48" t="n">
-        <v>10</v>
+        <v>2.5</v>
+      </c>
+      <c r="L48" t="n">
+        <v>90</v>
       </c>
       <c r="M48" t="n">
-        <v>12800</v>
+        <v>3200</v>
       </c>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr"/>
@@ -2870,13 +2900,13 @@
         </is>
       </c>
       <c r="K49" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L49" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M49" t="n">
-        <v>12400</v>
+        <v>3100</v>
       </c>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr"/>
@@ -2921,13 +2951,13 @@
         </is>
       </c>
       <c r="K50" t="n">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="L50" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="M50" t="n">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr"/>
@@ -2972,13 +3002,10 @@
         </is>
       </c>
       <c r="K51" t="n">
-        <v>10</v>
-      </c>
-      <c r="L51" t="n">
-        <v>110</v>
+        <v>2.5</v>
       </c>
       <c r="M51" t="n">
-        <v>11800</v>
+        <v>2950</v>
       </c>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr"/>
@@ -3023,13 +3050,10 @@
         </is>
       </c>
       <c r="K52" t="n">
-        <v>10</v>
-      </c>
-      <c r="L52" t="n">
-        <v>105</v>
+        <v>2.5</v>
       </c>
       <c r="M52" t="n">
-        <v>11500</v>
+        <v>2875</v>
       </c>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr"/>

</xml_diff>